<commit_message>
.: CLONE - Add Item Type Concept into website (WSM-129)
</commit_message>
<xml_diff>
--- a/src/assets/template/wonder-scale-template.xlsx
+++ b/src/assets/template/wonder-scale-template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edward\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Wonder Scale\wonder-scale-merchant\src\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -51,17 +51,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="2" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,9 +80,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -374,36 +366,36 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>9.8000000000000007</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>